<commit_message>
dataprovider test using excel data
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">title</t>
+    <t xml:space="preserve">first_name</t>
   </si>
   <si>
-    <t xml:space="preserve">firstname</t>
+    <t xml:space="preserve">second_name</t>
   </si>
   <si>
-    <t xml:space="preserve">lastname</t>
+    <t xml:space="preserve">f1</t>
   </si>
   <si>
-    <t xml:space="preserve">company</t>
+    <t xml:space="preserve">l1</t>
   </si>
 </sst>
 </file>
@@ -46,6 +46,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -105,8 +106,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -127,28 +132,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>